<commit_message>
GUI and importer fixes
</commit_message>
<xml_diff>
--- a/import/Kontoutdrag_exempel.xlsx
+++ b/import/Kontoutdrag_exempel.xlsx
@@ -1011,7 +1011,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Okategoriserad</t>
+          <t>Övriga inkomster</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1991,7 +1991,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Okategoriserad</t>
+          <t>Övrigt</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">

</xml_diff>